<commit_message>
updated order sheet formatting
</commit_message>
<xml_diff>
--- a/prep_and_checklists/Coulter Kunzel Memorial/Coulter Kunzel Memorial_2025-04-23_0.xlsx
+++ b/prep_and_checklists/Coulter Kunzel Memorial/Coulter Kunzel Memorial_2025-04-23_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcuvin/purveyor_project/prep_and_checklists/Coulter Kunzel Memorial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592FDA68-DC2F-C54D-B15E-9019C7BD72F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{133E7D4F-E969-6F4A-98C6-630482434E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15420" yWindow="760" windowWidth="30240" windowHeight="18040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="840" windowWidth="30240" windowHeight="17820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="prep_sheet" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="125">
   <si>
     <t>Coulter Kunzel Memorial Guest Count: N/A Guests Event Start Time: 12:00 PM Event End Time: 4:00 PM</t>
   </si>
@@ -353,12 +353,6 @@
     <t>Slice Rye Pullman</t>
   </si>
   <si>
-    <t>Cut chives</t>
-  </si>
-  <si>
-    <t>Whipped creme fraiche</t>
-  </si>
-  <si>
     <t>Smoked Salmon</t>
   </si>
   <si>
@@ -389,9 +383,6 @@
     <t>1 case</t>
   </si>
   <si>
-    <t>6 quarts</t>
-  </si>
-  <si>
     <t>2x sides</t>
   </si>
   <si>
@@ -399,6 +390,12 @@
   </si>
   <si>
     <t>QS</t>
+  </si>
+  <si>
+    <t>6 quarts, *approx 6 airliner brests</t>
+  </si>
+  <si>
+    <t>Whipped chive creme fraiche</t>
   </si>
 </sst>
 </file>
@@ -797,10 +794,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28:D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -809,6 +809,7 @@
     <col min="2" max="2" width="26.83203125" customWidth="1"/>
     <col min="4" max="4" width="41.33203125" customWidth="1"/>
     <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -820,6 +821,9 @@
       <c r="A4" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="D4" s="4" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -846,7 +850,7 @@
         <v>101</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="19" x14ac:dyDescent="0.2">
@@ -860,7 +864,7 @@
         <v>102</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="19" x14ac:dyDescent="0.2">
@@ -888,7 +892,7 @@
         <v>104</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="19" x14ac:dyDescent="0.2">
@@ -932,7 +936,7 @@
         <v>105</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="19" x14ac:dyDescent="0.2">
@@ -946,7 +950,7 @@
         <v>106</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="19" x14ac:dyDescent="0.2">
@@ -960,17 +964,17 @@
         <v>107</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="40" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="D17" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>122</v>
+      <c r="E17" s="5" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="20" x14ac:dyDescent="0.2">
@@ -1003,7 +1007,7 @@
         <v>109</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="19" x14ac:dyDescent="0.2">
@@ -1014,24 +1018,24 @@
         <v>82</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="3" t="s">
         <v>110</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>81</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="19" x14ac:dyDescent="0.2">
@@ -1040,12 +1044,6 @@
       </c>
       <c r="B23" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="19" x14ac:dyDescent="0.2">
@@ -1088,10 +1086,10 @@
         <v>79</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="19" x14ac:dyDescent="0.2">
@@ -1102,10 +1100,10 @@
         <v>84</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="19" x14ac:dyDescent="0.2">
@@ -1116,20 +1114,20 @@
         <v>71</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="19" x14ac:dyDescent="0.2">
@@ -1326,7 +1324,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup scale="61" orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -1567,5 +1565,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>